<commit_message>
DesignNotes for fleetmanager upload
</commit_message>
<xml_diff>
--- a/DesignNotes.xlsx
+++ b/DesignNotes.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProjects\fleetsaas\project_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D0BA5E-609C-4908-BC42-FBD46C850F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E795CAFD-A79B-4084-A38D-0AE209CFDCA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{BC5D643C-CD35-4DCC-AC35-EDA2DC25901C}"/>
+    <workbookView xWindow="57480" yWindow="14250" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{BC5D643C-CD35-4DCC-AC35-EDA2DC25901C}"/>
   </bookViews>
   <sheets>
     <sheet name="Roles" sheetId="1" r:id="rId1"/>
-    <sheet name="Design Session1-UserLogin" sheetId="2" r:id="rId2"/>
+    <sheet name="DBCredentials" sheetId="5" r:id="rId2"/>
+    <sheet name="DesignSess2-FleetManagerUpload" sheetId="6" r:id="rId3"/>
+    <sheet name="Design Session1-UserLogin" sheetId="2" r:id="rId4"/>
+    <sheet name="Bidding process" sheetId="4" r:id="rId5"/>
+    <sheet name="Country Cd" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
   <si>
     <t>HR Manager</t>
   </si>
@@ -82,6 +86,92 @@
     </r>
   </si>
   <si>
+    <t>1) Inserting a record  into user table with "Awaiting Approval" from backend
+2) Email generated to the approver with approval link
+3) Upon approval, update the status as Active on the user table &amp; generate a random password and send it to the user email.</t>
+  </si>
+  <si>
+    <t>Backend Steps</t>
+  </si>
+  <si>
+    <t>User Action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User </t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Users(Fleet, HR, Bidder)</t>
+  </si>
+  <si>
+    <t>User will login for the first time temporary password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On the onboard form - upon clicking the submit
+</t>
+  </si>
+  <si>
+    <t>UI would need role details, In the Reset API response from backend.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">APIs: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+  Login API</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>APIs:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+  Reset API
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Backend should inform UI if the last logged in is empty indicating that user is logging in for the first time</t>
+  </si>
+  <si>
+    <t>User logs into the system with a prompt to reset the password for the first time 
+     --&gt; User is shown the appropriate dashboard/view based on the role</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -102,7 +192,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-   User Table with columns; User name, Email address, Password, Role, Permission, Active status, created_on, created_by, approved_by, updated_by,     updated_on, Last logged in.
+   User Table with columns; User name, Email address, Password, Role, Permission, Active status, created_on, created_by, approved_by, updated_by,   updated_on, Last logged in.
 </t>
     </r>
     <r>
@@ -129,90 +219,131 @@
     </r>
   </si>
   <si>
-    <t>1) Inserting a record  into user table with "Awaiting Approval" from backend
-2) Email generated to the approver with approval link
-3) Upon approval, update the status as Active on the user table &amp; generate a random password and send it to the user email.</t>
-  </si>
-  <si>
-    <t>Backend Steps</t>
-  </si>
-  <si>
-    <t>User Action</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User </t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>Users(Fleet, HR, Bidder)</t>
-  </si>
-  <si>
-    <t>User will login for the first time temporary password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">On the onboard form - upon clicking the submit
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Country CD</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Upload request file</t>
+  </si>
+  <si>
+    <t>Add requests to request table</t>
+  </si>
+  <si>
+    <t>host: "64.225.28.128",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "user": "postgres",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "password": "rbadmin@RB123",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "name": "fleetmanager",</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>FileUpload</t>
+  </si>
+  <si>
+    <t>Uploaded</t>
+  </si>
+  <si>
+    <t>Reviewed</t>
+  </si>
+  <si>
+    <t>Submitted</t>
+  </si>
+  <si>
+    <t>Usecase1</t>
+  </si>
+  <si>
+    <t>Fleetmanager uploads an excel</t>
+  </si>
+  <si>
+    <t>In progress - Awaiting Response</t>
+  </si>
+  <si>
+    <t>Awaiting Response</t>
+  </si>
+  <si>
+    <t>In progress - Partial Bid Received</t>
+  </si>
+  <si>
+    <t>Partrially Bid received</t>
+  </si>
+  <si>
+    <t>Fullfilled</t>
+  </si>
+  <si>
+    <t>Systematically choose the lowest bid</t>
+  </si>
+  <si>
+    <t>Unfullfilled</t>
+  </si>
+  <si>
+    <t>FleetManager</t>
+  </si>
+  <si>
+    <t>Uploads a file with orders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) .csv file format
+2) UI to send uploaded file (.csv) throught the bulk upload api
+3) API to run validations
+4) if all passes: DB entries are made, success response sent back to UI: 
+ -&gt; Records are added to request table.
+ -&gt; Request # format: ORD-[Country 3characters]-[YYMMDDNNNNN]
+      For example: ORD-USA-24021112345
+ -&gt; Status: Uploaded
+5) if there is failure: reject the entire file &amp; show the problematic record(s)
 </t>
   </si>
   <si>
-    <t>UI would need role details, In the Reset API response from backend.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">APIs: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-  Login API</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>APIs:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-  Reset API
+    <t>APIs: upload
+Tables: request &amp; request_status</t>
+  </si>
+  <si>
+    <t>Submit for Bidding</t>
+  </si>
+  <si>
+    <t>Review the uploaded records</t>
+  </si>
+  <si>
+    <t>API: update_request (for any final edits)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) UI must show a button to review and edit.
+2) FM clicks on the review button -&gt; Status: Reviewed
 </t>
-    </r>
-  </si>
-  <si>
-    <t>Backend should inform UI if the last logged in is empty indicating that user is logging in for the first time</t>
-  </si>
-  <si>
-    <t>User logs into the system with a prompt to reset the password for the first time 
-     --&gt; User is shown the appropriate dashboard/view based on the role</t>
+  </si>
+  <si>
+    <t>API: submit_bid</t>
+  </si>
+  <si>
+    <t>3) FM releases it for bidding -&gt; Status: Submitted
+4) bid requests  sent to 3 bidders for action</t>
+  </si>
+  <si>
+    <t>requirements captured below</t>
+  </si>
+  <si>
+    <t>Validation Rules</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -236,7 +367,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -258,6 +389,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -315,9 +452,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,11 +864,247 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805C65B9-A644-4A2D-83C5-E81219998B8E}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="28.89453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{752F1C3D-5E08-4421-BA38-A6BE918E036A}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="14.83984375" customWidth="1"/>
+    <col min="2" max="2" width="31.3671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.89453125" customWidth="1"/>
+    <col min="4" max="4" width="44.3125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="9">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="9"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="129.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685626B0-E786-43A5-8CCB-01BF72D0C352}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -720,25 +1112,25 @@
     <col min="1" max="1" width="19.3125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56.734375" style="5" customWidth="1"/>
     <col min="3" max="3" width="54.1015625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.7890625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="59.15625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.83984375" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>9</v>
@@ -746,44 +1138,44 @@
     </row>
     <row r="4" spans="1:4" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>18</v>
-      </c>
       <c r="C5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -792,4 +1184,77 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7232DDF4-A8D3-401E-8D56-42B36EDD387F}">
+  <dimension ref="A2:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="4.62890625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="26.20703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E02243C-26B1-4F7A-9633-1A83C9335DF2}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="7.578125" customWidth="1"/>
+    <col min="2" max="2" width="10.3671875" customWidth="1"/>
+    <col min="3" max="3" width="10.41796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>